<commit_message>
Updated GENDER extraction scripts
</commit_message>
<xml_diff>
--- a/extracted_excel/Baringo_gendered_enterprise.xlsx
+++ b/extracted_excel/Baringo_gendered_enterprise.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
-  <si>
-    <t>County</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>Theme</t>
   </si>
@@ -28,9 +25,6 @@
     <t>Response</t>
   </si>
   <si>
-    <t>Baringo</t>
-  </si>
-  <si>
     <t>Enterprise Selection and Community Involvement</t>
   </si>
   <si>
@@ -190,7 +184,7 @@
     <t>Baringo county has competitive advantage in the north rift region in the production of goat meat. Baringo has extensive land mass and conducive climate for goat rearing. The participation of women in the value chain is production and dairy goat milk products</t>
   </si>
   <si>
-    <t>value chain(product) Economic benefits and profitability levels coffee high milk Moderate meat low vegetables High chicken meat High fish low mangoes medium Ground nuts High Green maize High</t>
+    <t>coffee high milk Moderate meat low vegetables High chicken meat High fish low mangoes medium Ground nuts High Green maize High</t>
   </si>
   <si>
     <t>The enterprise turn over is low but sustainable. market accessibility and availability is high it is less vulnerable to climate variabilities</t>
@@ -199,9 +193,6 @@
     <t>Majorly improves household welfare and nutrition</t>
   </si>
   <si>
-    <t>No response provided</t>
-  </si>
-  <si>
     <t>Yes; climatic conditions dictates the suitability of the enterprise</t>
   </si>
   <si>
@@ -211,6 +202,9 @@
     <t>County Departmental reports ( No specific survey reports)</t>
   </si>
   <si>
+    <t>no policy framework</t>
+  </si>
+  <si>
     <t>Women based farmer groups are not registered as cooperatives. The operational does support agricultural enterprise development.</t>
   </si>
   <si>
@@ -223,7 +217,7 @@
     <t>No specific existing policies governing these form of enterprises.</t>
   </si>
   <si>
-    <t>Policy development to regulate enterprise operations capacity build ToTs to offer technical support to organized groups - mentoring and networking. offer technology and digital literacy Improve access to financial resources [UNLINKED TABLE DATA]: value chain(product) | market demand coffee | high milk | high meat | high vegetables | medium chicken meat | low fish | low mangoes | medium [UNLINKED TABLE DATA]: value chain(product) | Economic benefits and profitability levels coffee | high milk | Moderate meat | low vegetables | High chicken meat | High fish | low mangoes | medium Ground nuts | High Green maize | High</t>
+    <t>Policy development to regulate enterprise operations capacity build ToTs to offer technical support to organized groups - mentoring and networking. offer technology and digital literacy Improve access to financial resources</t>
   </si>
 </sst>
 </file>
@@ -581,13 +575,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,414 +591,321 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
         <v>38</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C30" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>